<commit_message>
solicitud gráfica tema 1 grado 10
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/SolicitudGrafica-MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/SolicitudGrafica-MA_08_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA\Octavo\MA_08_01_CO\MA_08_01_CO_revisión de estilo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="173">
   <si>
     <t>Fecha:</t>
   </si>
@@ -513,9 +513,6 @@
     <t>Josué Malagón</t>
   </si>
   <si>
-    <t>Los Números reales propiedades y operaciones</t>
-  </si>
-  <si>
     <t>Ilustración</t>
   </si>
   <si>
@@ -528,21 +525,9 @@
     <t>Cuaderno de Estudio</t>
   </si>
   <si>
-    <t>Una manzana partida en 4 partes, las cuatro partes sumadas son iguales a una manzana.</t>
-  </si>
-  <si>
-    <t>El color del fondo de la imagen se puede quitar para que no quede un cuadro.</t>
-  </si>
-  <si>
     <t>IMG02</t>
   </si>
   <si>
-    <t>Pie de rey digital que esta tomando la medida del ancho o largo de un objeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El pie de rey debe estar midiendo el ancho de un borrador y el tablero digital debe marcar una medida de 15.73 mm </t>
-  </si>
-  <si>
     <t>IMG03</t>
   </si>
   <si>
@@ -564,43 +549,116 @@
     <t>IMG09</t>
   </si>
   <si>
-    <t>Resaltar los números irracionales.</t>
-  </si>
-  <si>
     <t>IMG10</t>
   </si>
   <si>
     <t>IMG11</t>
   </si>
   <si>
-    <t>Se busca resaltar como el conjunto de los números reales contiene a otros subconjuntos numéricos.</t>
-  </si>
-  <si>
     <t>IMG12</t>
   </si>
   <si>
-    <t xml:space="preserve">Construir una imagen similar a la de la siguiente URL: http://2.bp.blogspot.com/-UXYpA2xs1rc/UPmW-1bXItI/AAAAAAAAABI/uKgOOFvBWPE/s400/graficanumreales.gif  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construir una imagen similar a la que se encuentra en la siguiente URL: http://upload.wikimedia.org/wikipedia/commons/thumb/9/93/Number-line.svg/750px-Number-line.svg.png  </t>
-  </si>
-  <si>
-    <t>Se desea resaltar que los espacioes entre los números enteros están ocupados por los demas números reales.</t>
-  </si>
-  <si>
-    <t>MA_08_01_CO</t>
-  </si>
-  <si>
     <t>IMG14</t>
   </si>
   <si>
     <t>IMG13</t>
   </si>
   <si>
-    <t xml:space="preserve">Se muestra un pequeño mapa conceptual de los conjuntos numéricos. </t>
-  </si>
-  <si>
-    <t>número irracional de gran importancia.</t>
+    <t>MA_10_01_CO</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>Crear un par de conjuntos M (de Madres) y H (de Hijos) y una relación entre conjuntos como la que se puede ver en observaciones, en la que Mercedes es madre de Carlos, Laura y Mauricio, Gilma es madre de Diana, César y Rubén, mientras que Alicia es madre de Rocío. Así, en el conjunto M están Mercedes, Gilma y Alicia, mientras que en el conjunto H están todos los demás.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear un par de conjuntos D (de Diagonales) y P (de Polígonos) y una relación entre conjuntos como la que se muestra en observaciones, En la que a cada tipo de polígono, se le asigna la cantidad de diagonales correspondiente.
+NO OLVIDAR: Cambiar los nombres de los conjuntos.
+NO OLVIDAR: Incluir el número 0 y el 1 en el conjunto de números.
+NO OLVIDAR: Incluir polígonos cóncavos y no regulares.
+Los triángulos tendrán correspondencia con el 0
+Los cuadriláteros con el 2,
+Los pentágonos con el 5,
+Los hexágonos con el 9 y, en general, un polígono de n lados con el número n(n-3)/2
+El conjunto de salida siempre ponerlo en color rojo, y el llegada en color azul.
+ </t>
+  </si>
+  <si>
+    <t>La imagen debe quedar muy similar a la siguiente, FAVOR HACER VERDES LAS FLECHAS, La selección de colores rojo y azul para los conjuntos de salida y llegada y de verde o naranja no es arbitraria, se usa todo el tiempo para identificar DominIo, codominio y Rango, además para identificar la ubicación de los conjuntos en las diferentes representaciones</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Del mismo modo que en la imagen, dejar el mismo conjunto de partida N rojo, pero en el de llegada poner los respectivos números de Fibonacci. (Es decir , el listado azul es </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3366FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1,1, 2, 3, 5, 8, 13, 21, 34, 55,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3366FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>377</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3366FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>610 y 196418</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">). No olvidar: poner en desorden los números de Fibonacci.
+Hacer VERDES las flechas de asignación
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Crear una representación entre dos conjuntos N y C, no ordenados de números naturales y cuadrados, con sus correspondencias puestas como flechas (VERDES), como l que se ve en observaciones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esta gráfica se construyó como una captura de pantalla desde el archivo de Geogebra que indica el tránsito entre la representación conjuntista y la gráfica de la función y=f(x)=xcuadrado; MANTENER los colores de la gráfica de ejemplo y colocar los nombres de los ejes del plano cartesiano en mayúscula e itálica. </t>
+  </si>
+  <si>
+    <t>LA X y la Y deben ser en itálica y mayúscula.</t>
+  </si>
+  <si>
+    <t>Cambiar el color de los conjuntos y las flechas: X rojo, Y azul y las flechas verdes.</t>
   </si>
 </sst>
 </file>
@@ -610,7 +668,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -760,6 +818,25 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3366FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFDE9400"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1311,7 +1388,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1599,6 +1676,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1716,7 +1802,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1733,304 +1819,78 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2174875</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\FAMILIA\Documents\planeta\Autor\Racionales 1.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13991167" y="2645833"/>
-          <a:ext cx="2174875" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2179955</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 4" descr="C:\Users\FAMILIA\AppData\Local\Temp\geogebra.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13991167" y="3206750"/>
-          <a:ext cx="2179955" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2179320</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>359142</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 5" descr="C:\Users\FAMILIA\Documents\planeta\Autor\imagenes\orden1.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13991167" y="3577167"/>
-          <a:ext cx="2179320" cy="359142"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2176145</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4233</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 6" descr="C:\Users\FAMILIA\Documents\planeta\Autor\imagenes\orden2.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13991167" y="3947583"/>
-          <a:ext cx="2176145" cy="342900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2174875</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>347345</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 7" descr="C:\Users\FAMILIA\Documents\planeta\Autor\imagenes\orden3.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13991167" y="4286250"/>
-          <a:ext cx="2174875" cy="347345"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>116416</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2176780" cy="346075"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 8" descr="C:\Users\FAMILIA\Documents\planeta\Autor\imagenes\irracional.png"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14276917" y="8879416"/>
-          <a:ext cx="2176780" cy="346075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>137584</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>836083</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>1962150</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>1581150</xdr:rowOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>699559</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>2321983</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3076" name="Object 4" hidden="1">
+            <xdr:cNvPr id="3079" name="Object 7" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s3076"/>
+                  <a14:compatExt spid="_x0000_s3079"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>438150</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>2143125</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3080" name="Object 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2063,34 +1923,38 @@
   </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2333357</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>488527</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2139690</xdr:rowOff>
+      <xdr:rowOff>1922145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14181667" y="2709333"/>
-          <a:ext cx="2142857" cy="2076190"/>
+          <a:off x="20118917" y="7291917"/>
+          <a:ext cx="2562860" cy="1922145"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2099,57 +1963,394 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>84668</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>63502</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>1788583</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>777704</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3077" name="Object 5" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s3077"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>312632</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20118917" y="9461500"/>
+          <a:ext cx="2386965" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6117167</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2063327</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1555750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20108334" y="11684000"/>
+          <a:ext cx="2073910" cy="1555750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2462530</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2462530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagen 15"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13991167" y="13832417"/>
+          <a:ext cx="2462530" cy="2462530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2995930</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1312545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagen 17"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13991167" y="16562917"/>
+          <a:ext cx="2995930" cy="1312545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1689100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1570990</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagen 18"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13991167" y="19399250"/>
+          <a:ext cx="1689100" cy="1570990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2091055</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3042920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagen 19"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13991167" y="21124333"/>
+          <a:ext cx="2091055" cy="3042920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2676525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1189355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagen 20"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13991167" y="24278167"/>
+          <a:ext cx="2676525" cy="1189355"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1657985</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1608455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagen 21"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13991167" y="25548167"/>
+          <a:ext cx="1657985" cy="1608455"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2565400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2722245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagen 22"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13991167" y="27410833"/>
+          <a:ext cx="2565400" cy="2722245"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2868,9 +3069,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2926,7 +3127,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="87">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="88"/>
       <c r="F3" s="80"/>
@@ -2941,7 +3142,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="5"/>
@@ -2949,7 +3150,7 @@
         <v>55</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -2997,7 +3198,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>39</v>
@@ -3064,27 +3265,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="26">
-        <v>141122494</v>
+      <c r="B10" s="26" t="s">
+        <v>148</v>
       </c>
       <c r="C10" s="26" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_08_01_CO_IMG01_small</v>
+        <v>MA_10_01_CO_IMG01_small</v>
       </c>
       <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3092,39 +3293,37 @@
       </c>
       <c r="H10" s="14" t="str">
         <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG01_zoom</v>
+        <v>MA_10_01_CO_IMG01_zoom</v>
       </c>
       <c r="I10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="27">
-        <v>251995600</v>
+        <v>150</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>148</v>
       </c>
       <c r="C11" s="26" t="str">
         <f t="shared" ref="C11:C18" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F75" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_08_01_CO_IMG02_small</v>
+        <v>MA_10_01_CO_IMG02_small</v>
       </c>
       <c r="G11" s="14" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3132,39 +3331,37 @@
       </c>
       <c r="H11" s="14" t="str">
         <f t="shared" ref="H11:H75" si="2">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG02_zoom</v>
+        <v>MA_10_01_CO_IMG02_zoom</v>
       </c>
       <c r="I11" s="14" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>155</v>
-      </c>
+      <c r="J11" s="110" t="s">
+        <v>166</v>
+      </c>
+      <c r="K11"/>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG03_small</v>
+        <v>MA_10_01_CO_IMG03_small</v>
       </c>
       <c r="G12" s="14" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3172,37 +3369,37 @@
       </c>
       <c r="H12" s="14" t="str">
         <f t="shared" ref="H12" si="3">IF(AND(I12&lt;&gt;"",I12&lt;&gt;0),IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG03_zoom</v>
+        <v>MA_10_01_CO_IMG03_zoom</v>
       </c>
       <c r="I12" s="14" t="str">
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="77" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="109" t="s">
+        <v>167</v>
+      </c>
+      <c r="K12" s="77"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG04_small</v>
+        <v>MA_10_01_CO_IMG04_small</v>
       </c>
       <c r="G13" s="14" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3210,35 +3407,37 @@
       </c>
       <c r="H13" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG04_zoom</v>
+        <v>MA_10_01_CO_IMG04_zoom</v>
       </c>
       <c r="I13" s="14" t="str">
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="19"/>
+      <c r="J13" s="110" t="s">
+        <v>168</v>
+      </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG05_small</v>
+        <v>MA_10_01_CO_IMG05_small</v>
       </c>
       <c r="G14" s="14" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3246,34 +3445,36 @@
       </c>
       <c r="H14" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG05_zoom</v>
+        <v>MA_10_01_CO_IMG05_zoom</v>
       </c>
       <c r="I14" s="14" t="str">
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14"/>
+      <c r="J14" s="77" t="s">
+        <v>169</v>
+      </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B15" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>150</v>
-      </c>
       <c r="D15" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG06_small</v>
+        <v>MA_10_01_CO_IMG06_small</v>
       </c>
       <c r="G15" s="14" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3281,35 +3482,37 @@
       </c>
       <c r="H15" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG06_zoom</v>
+        <v>MA_10_01_CO_IMG06_zoom</v>
       </c>
       <c r="I15" s="14" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="109" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG07_small</v>
+        <v>MA_10_01_CO_IMG07_small</v>
       </c>
       <c r="G16" s="14" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3317,35 +3520,37 @@
       </c>
       <c r="H16" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG07_zoom</v>
+        <v>MA_10_01_CO_IMG07_zoom</v>
       </c>
       <c r="I16" s="14" t="str">
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="111" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG08_small</v>
+        <v>MA_10_01_CO_IMG08_small</v>
       </c>
       <c r="G17" s="14" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3353,7 +3558,7 @@
       </c>
       <c r="H17" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG08_zoom</v>
+        <v>MA_10_01_CO_IMG08_zoom</v>
       </c>
       <c r="I17" s="14" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3362,26 +3567,26 @@
       <c r="J17" s="31"/>
       <c r="K17" s="34"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>MA_08_01_CO_IMG09_small</v>
+        <v>MA_10_01_CO_IMG09_small</v>
       </c>
       <c r="G18" s="14" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3389,7 +3594,7 @@
       </c>
       <c r="H18" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>MA_08_01_CO_IMG09_zoom</v>
+        <v>MA_10_01_CO_IMG09_zoom</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3398,26 +3603,26 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="26" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I19="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_08_01_CO_IMG10_small</v>
+        <v>MA_10_01_CO_IMG10_small</v>
       </c>
       <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3425,7 +3630,7 @@
       </c>
       <c r="H19" s="14" t="str">
         <f>IF(AND(I19&lt;&gt;"",I19&lt;&gt;0),IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE($C$7,"_",$A19,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG10_zoom</v>
+        <v>MA_10_01_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3433,12 +3638,12 @@
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B20" s="27">
         <v>189851069</v>
@@ -3448,14 +3653,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F20" s="14" t="str">
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE($C$7,"_",$A20,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I20="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_08_01_CO_IMG11_small</v>
+        <v>MA_10_01_CO_IMG11_small</v>
       </c>
       <c r="G20" s="14" t="str">
         <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3463,37 +3668,35 @@
       </c>
       <c r="H20" s="14" t="str">
         <f>IF(AND(I20&lt;&gt;"",I20&lt;&gt;0),IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE($C$7,"_",$A20,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG11_zoom</v>
+        <v>MA_10_01_CO_IMG11_zoom</v>
       </c>
       <c r="I20" s="14" t="str">
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="20" t="s">
-        <v>175</v>
-      </c>
+      <c r="J20" s="20"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="12" customFormat="1" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="26" t="str">
         <f t="shared" ref="C21:C23" si="4">IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F21" s="14" t="str">
         <f t="shared" ref="F21:F23" si="5">IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE($C$7,"_",$A21,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I21="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_08_01_CO_IMG12_small</v>
+        <v>MA_10_01_CO_IMG12_small</v>
       </c>
       <c r="G21" s="14" t="str">
         <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3501,7 +3704,7 @@
       </c>
       <c r="H21" s="14" t="str">
         <f t="shared" ref="H21:H23" si="6">IF(AND(I21&lt;&gt;"",I21&lt;&gt;0),IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),CONCATENATE($C$7,"_",$A21,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>MA_08_01_CO_IMG12_zoom</v>
+        <v>MA_10_01_CO_IMG12_zoom</v>
       </c>
       <c r="I21" s="14" t="str">
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3510,26 +3713,26 @@
       <c r="J21" s="31"/>
       <c r="K21" s="34"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" s="26" t="str">
         <f t="shared" si="4"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>MA_08_01_CO_IMG13_small</v>
+        <v>MA_10_01_CO_IMG13_small</v>
       </c>
       <c r="G22" s="14" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3537,39 +3740,35 @@
       </c>
       <c r="H22" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>MA_08_01_CO_IMG13_zoom</v>
+        <v>MA_10_01_CO_IMG13_zoom</v>
       </c>
       <c r="I22" s="14" t="str">
         <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="J22" s="19"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" s="26" t="str">
         <f t="shared" si="4"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>MA_08_01_CO_IMG14_small</v>
+        <v>MA_10_01_CO_IMG14_small</v>
       </c>
       <c r="G23" s="14" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3577,18 +3776,14 @@
       </c>
       <c r="H23" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>MA_08_01_CO_IMG14_zoom</v>
+        <v>MA_10_01_CO_IMG14_zoom</v>
       </c>
       <c r="I23" s="14" t="str">
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>170</v>
-      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="str">
@@ -5821,52 +6016,52 @@
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="3076" r:id="rId4">
+        <oleObject progId="PBrush" shapeId="3079" r:id="rId4">
           <objectPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>133350</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>838200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>1962150</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>1581150</xdr:rowOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>695325</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>2324100</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="3076" r:id="rId4"/>
+        <oleObject progId="PBrush" shapeId="3079" r:id="rId4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="3077" r:id="rId6">
+        <oleObject progId="PBrush" shapeId="3080" r:id="rId6">
           <objectPr defaultSize="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>1790700</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>781050</xdr:rowOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>438150</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>2143125</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="3077" r:id="rId6"/>
+        <oleObject progId="PBrush" shapeId="3080" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>